<commit_message>
Chore: Organize the data in an Excel.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Documents\GitHub\masterthesisSecret\steps\The actual project\content to commit\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93888FF-C383-4A20-AC5A-AB76270A68BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,70 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+  <si>
+    <t>Testing Epochs Scenario</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>MAE Latitude</t>
+  </si>
+  <si>
+    <t>MAE Longitude</t>
+  </si>
+  <si>
+    <t>RMSE Latitude</t>
+  </si>
+  <si>
+    <t>RMSE Longitude</t>
+  </si>
+  <si>
+    <t>Testing Units Scenario</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Testing Activations Scenario</t>
+  </si>
+  <si>
+    <t>Activation</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Sigmoid</t>
+  </si>
+  <si>
+    <t>SoftPlus</t>
+  </si>
+  <si>
+    <t>Tahn</t>
+  </si>
+  <si>
+    <t>Testing Anticipation Scenario</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>cyclic</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +398,364 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>8.2970719840127993E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.32484734962200101</v>
+      </c>
+      <c r="D3">
+        <v>0.18266855782366301</v>
+      </c>
+      <c r="E3">
+        <v>0.66924734465049096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>1.5463259035930699E-2</v>
+      </c>
+      <c r="C4">
+        <v>2.01952469303745E-2</v>
+      </c>
+      <c r="D4">
+        <v>9.6258813483183894E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.18485064806864801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>500</v>
+      </c>
+      <c r="B5">
+        <v>3.1050545169861901E-2</v>
+      </c>
+      <c r="C5">
+        <v>2.2311802088196098E-2</v>
+      </c>
+      <c r="D5">
+        <v>7.1753596482378099E-2</v>
+      </c>
+      <c r="E5">
+        <v>0.14191837441041599</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1000</v>
+      </c>
+      <c r="B6">
+        <v>9.18616152861392E-3</v>
+      </c>
+      <c r="C6">
+        <v>2.91620273138989E-2</v>
+      </c>
+      <c r="D6">
+        <v>6.1132870772399699E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.107507907705538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>9.18616152861392E-3</v>
+      </c>
+      <c r="C11">
+        <v>2.91620273138989E-2</v>
+      </c>
+      <c r="D11">
+        <v>6.1132870772399699E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.107507907705538</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>2.29251242959886E-2</v>
+      </c>
+      <c r="C12">
+        <v>2.6419629111345301E-2</v>
+      </c>
+      <c r="D12">
+        <v>7.5781045442915501E-2</v>
+      </c>
+      <c r="E12">
+        <v>6.14849283177831E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>500</v>
+      </c>
+      <c r="B13">
+        <v>2.3442447640723799E-2</v>
+      </c>
+      <c r="C13">
+        <v>3.7877987407419003E-2</v>
+      </c>
+      <c r="D13">
+        <v>7.7182472534437593E-2</v>
+      </c>
+      <c r="E13">
+        <v>7.1557683886921603E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1000</v>
+      </c>
+      <c r="B14">
+        <v>8.7985649010277299E-3</v>
+      </c>
+      <c r="C14">
+        <v>6.3664978495458699E-2</v>
+      </c>
+      <c r="D14">
+        <v>5.7300794077937998E-2</v>
+      </c>
+      <c r="E14">
+        <v>8.5361579095533394E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>9.18616152861392E-3</v>
+      </c>
+      <c r="C19">
+        <v>2.91620273138989E-2</v>
+      </c>
+      <c r="D19">
+        <v>6.1132870772399699E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.107507907705538</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>1.29764720936017E-2</v>
+      </c>
+      <c r="C20">
+        <v>6.38223918333826E-3</v>
+      </c>
+      <c r="D20">
+        <v>4.3596487969186297E-2</v>
+      </c>
+      <c r="E20">
+        <v>2.6846473065442401E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>9.6779705392663704E-3</v>
+      </c>
+      <c r="C21">
+        <v>5.86969380989811E-3</v>
+      </c>
+      <c r="D21">
+        <v>5.1010822072126698E-2</v>
+      </c>
+      <c r="E21">
+        <v>2.6711359071230199E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>1.0367250064069199E-2</v>
+      </c>
+      <c r="C22">
+        <v>2.22531231519357E-2</v>
+      </c>
+      <c r="D22">
+        <v>4.7673735576762702E-2</v>
+      </c>
+      <c r="E22">
+        <v>7.1859023986932197E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>2.60999028932043E-2</v>
+      </c>
+      <c r="C23">
+        <v>1.3418703414070299E-2</v>
+      </c>
+      <c r="D23">
+        <v>5.0009259420673503E-2</v>
+      </c>
+      <c r="E23">
+        <v>2.92744594391776E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>9.18616152861392E-3</v>
+      </c>
+      <c r="C28">
+        <v>2.91620273138989E-2</v>
+      </c>
+      <c r="D28">
+        <v>6.1132870772399699E-2</v>
+      </c>
+      <c r="E28">
+        <v>0.107507907705538</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>1.51025068435228E-2</v>
+      </c>
+      <c r="C29">
+        <v>3.8248616113415998E-2</v>
+      </c>
+      <c r="D29">
+        <v>4.7979877606940599E-2</v>
+      </c>
+      <c r="E29">
+        <v>6.1632094677201599E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>